<commit_message>
Adding ramp costs to thermal units. Updating some major bugs (cb for other non-res blocking generation if no steam demand -> removing cb, demand reduction inputs and outputs were reversed, too small dr capacity in Germany) and few smaller ones.
</commit_message>
<xml_diff>
--- a/src_files/data_files/demanddata_DH_own_projection.xlsx
+++ b/src_files/data_files/demanddata_DH_own_projection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F23D3D6-66D5-414D-914E-D76755F066AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3B5B17-C1D2-4BDE-8210-0C18A47136EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" tabRatio="854" activeTab="1" xr2:uid="{3FAE13E1-8810-491E-8373-B01BC9956BE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="854" activeTab="1" xr2:uid="{3FAE13E1-8810-491E-8373-B01BC9956BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="14" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="POP" sheetId="2" r:id="rId11"/>
     <sheet name="HDD" sheetId="3" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1105,24 +1105,6 @@
     <t>NEBB</t>
   </si>
   <si>
-    <t>_HKI</t>
-  </si>
-  <si>
-    <t>_ESP</t>
-  </si>
-  <si>
-    <t>_VAN</t>
-  </si>
-  <si>
-    <t>_TRE</t>
-  </si>
-  <si>
-    <t>_OUL</t>
-  </si>
-  <si>
-    <t>_ROF</t>
-  </si>
-  <si>
     <t>Normal year net prod /  pers</t>
   </si>
   <si>
@@ -1268,10 +1250,28 @@
     <t>dheat</t>
   </si>
   <si>
-    <t>_TKU</t>
+    <t>HKI</t>
   </si>
   <si>
-    <t>_JKL</t>
+    <t>ESP</t>
+  </si>
+  <si>
+    <t>VAN</t>
+  </si>
+  <si>
+    <t>TKU</t>
+  </si>
+  <si>
+    <t>TRE</t>
+  </si>
+  <si>
+    <t>OUL</t>
+  </si>
+  <si>
+    <t>JKL</t>
+  </si>
+  <si>
+    <t>ROF</t>
   </si>
 </sst>
 </file>
@@ -25211,101 +25211,101 @@
   <sheetData>
     <row r="4" spans="2:4">
       <c r="B4" s="157" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="157" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="158" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="158" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="158" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="157" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="C12" s="158" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="D12" s="158" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="C13" s="158" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D13" s="158" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="C14" s="158" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D14" s="158" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="C15" s="158" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="D15" s="158" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="C16" s="158" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D16" s="158" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="C17" s="158" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D17" s="158" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="C18" s="158" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D18" s="158" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="157" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="C21" s="158" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D21" s="158" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -25313,87 +25313,87 @@
         <v>178</v>
       </c>
       <c r="D22" s="158" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="157" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="C26" s="158" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="C27" s="158" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="C28" s="158" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" s="158" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="158" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" s="158" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="157" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="36" spans="2:3">
       <c r="C36" s="158" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="37" spans="2:3">
       <c r="C37" s="158" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="39" spans="2:3">
       <c r="C39" s="158" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="40" spans="2:3">
       <c r="C40" s="158" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="42" spans="2:3">
       <c r="B42" s="157" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="43" spans="2:3">
       <c r="C43" s="158" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="44" spans="2:3">
       <c r="C44" s="158" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="45" spans="2:3">
       <c r="C45" s="158" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -40677,8 +40677,8 @@
   <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I81" sqref="I81"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40710,7 +40710,7 @@
         <v>175</v>
       </c>
       <c r="F1" s="151" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="G1" s="156" t="s">
         <v>176</v>
@@ -40727,7 +40727,7 @@
       </c>
       <c r="C2" t="str">
         <f>IF(Finland!D5="","",Finland!D5)</f>
-        <v>_HKI</v>
+        <v>HKI</v>
       </c>
       <c r="D2" t="str">
         <f>IF(Finland!E5="","",Finland!E5)</f>
@@ -40757,7 +40757,7 @@
       </c>
       <c r="C3" t="str">
         <f>IF(Finland!D6="","",Finland!D6)</f>
-        <v>_ESP</v>
+        <v>ESP</v>
       </c>
       <c r="D3" t="str">
         <f>IF(Finland!E6="","",Finland!E6)</f>
@@ -40787,7 +40787,7 @@
       </c>
       <c r="C4" t="str">
         <f>IF(Finland!D7="","",Finland!D7)</f>
-        <v>_VAN</v>
+        <v>VAN</v>
       </c>
       <c r="D4" t="str">
         <f>IF(Finland!E7="","",Finland!E7)</f>
@@ -40817,7 +40817,7 @@
       </c>
       <c r="C5" t="str">
         <f>IF(Finland!D8="","",Finland!D8)</f>
-        <v>_TKU</v>
+        <v>TKU</v>
       </c>
       <c r="D5" t="str">
         <f>IF(Finland!E8="","",Finland!E8)</f>
@@ -40847,7 +40847,7 @@
       </c>
       <c r="C6" t="str">
         <f>IF(Finland!D9="","",Finland!D9)</f>
-        <v>_TRE</v>
+        <v>TRE</v>
       </c>
       <c r="D6" t="str">
         <f>IF(Finland!E9="","",Finland!E9)</f>
@@ -40877,7 +40877,7 @@
       </c>
       <c r="C7" t="str">
         <f>IF(Finland!D10="","",Finland!D10)</f>
-        <v>_OUL</v>
+        <v>OUL</v>
       </c>
       <c r="D7" t="str">
         <f>IF(Finland!E10="","",Finland!E10)</f>
@@ -40907,7 +40907,7 @@
       </c>
       <c r="C8" t="str">
         <f>IF(Finland!D11="","",Finland!D11)</f>
-        <v>_JKL</v>
+        <v>JKL</v>
       </c>
       <c r="D8" t="str">
         <f>IF(Finland!E11="","",Finland!E11)</f>
@@ -40937,7 +40937,7 @@
       </c>
       <c r="C9" t="str">
         <f>IF(Finland!D12="","",Finland!D12)</f>
-        <v>_ROF</v>
+        <v>ROF</v>
       </c>
       <c r="D9" t="str">
         <f>IF(Finland!E12="","",Finland!E12)</f>
@@ -40967,7 +40967,7 @@
       </c>
       <c r="C10" t="str">
         <f>IF(Finland!D13="","",Finland!D13)</f>
-        <v>_HKI</v>
+        <v>HKI</v>
       </c>
       <c r="D10" t="str">
         <f>IF(Finland!E13="","",Finland!E13)</f>
@@ -40997,7 +40997,7 @@
       </c>
       <c r="C11" t="str">
         <f>IF(Finland!D14="","",Finland!D14)</f>
-        <v>_ESP</v>
+        <v>ESP</v>
       </c>
       <c r="D11" t="str">
         <f>IF(Finland!E14="","",Finland!E14)</f>
@@ -41027,7 +41027,7 @@
       </c>
       <c r="C12" t="str">
         <f>IF(Finland!D15="","",Finland!D15)</f>
-        <v>_VAN</v>
+        <v>VAN</v>
       </c>
       <c r="D12" t="str">
         <f>IF(Finland!E15="","",Finland!E15)</f>
@@ -41057,7 +41057,7 @@
       </c>
       <c r="C13" t="str">
         <f>IF(Finland!D16="","",Finland!D16)</f>
-        <v>_TKU</v>
+        <v>TKU</v>
       </c>
       <c r="D13" t="str">
         <f>IF(Finland!E16="","",Finland!E16)</f>
@@ -41087,7 +41087,7 @@
       </c>
       <c r="C14" t="str">
         <f>IF(Finland!D17="","",Finland!D17)</f>
-        <v>_TRE</v>
+        <v>TRE</v>
       </c>
       <c r="D14" t="str">
         <f>IF(Finland!E17="","",Finland!E17)</f>
@@ -41117,7 +41117,7 @@
       </c>
       <c r="C15" t="str">
         <f>IF(Finland!D18="","",Finland!D18)</f>
-        <v>_OUL</v>
+        <v>OUL</v>
       </c>
       <c r="D15" t="str">
         <f>IF(Finland!E18="","",Finland!E18)</f>
@@ -41147,7 +41147,7 @@
       </c>
       <c r="C16" t="str">
         <f>IF(Finland!D19="","",Finland!D19)</f>
-        <v>_JKL</v>
+        <v>JKL</v>
       </c>
       <c r="D16" t="str">
         <f>IF(Finland!E19="","",Finland!E19)</f>
@@ -41177,7 +41177,7 @@
       </c>
       <c r="C17" t="str">
         <f>IF(Finland!D20="","",Finland!D20)</f>
-        <v>_ROF</v>
+        <v>ROF</v>
       </c>
       <c r="D17" t="str">
         <f>IF(Finland!E20="","",Finland!E20)</f>
@@ -41207,7 +41207,7 @@
       </c>
       <c r="C18" t="str">
         <f>IF(Finland!D21="","",Finland!D21)</f>
-        <v>_HKI</v>
+        <v>HKI</v>
       </c>
       <c r="D18" t="str">
         <f>IF(Finland!E21="","",Finland!E21)</f>
@@ -41237,7 +41237,7 @@
       </c>
       <c r="C19" t="str">
         <f>IF(Finland!D22="","",Finland!D22)</f>
-        <v>_ESP</v>
+        <v>ESP</v>
       </c>
       <c r="D19" t="str">
         <f>IF(Finland!E22="","",Finland!E22)</f>
@@ -41267,7 +41267,7 @@
       </c>
       <c r="C20" t="str">
         <f>IF(Finland!D23="","",Finland!D23)</f>
-        <v>_VAN</v>
+        <v>VAN</v>
       </c>
       <c r="D20" t="str">
         <f>IF(Finland!E23="","",Finland!E23)</f>
@@ -41297,7 +41297,7 @@
       </c>
       <c r="C21" t="str">
         <f>IF(Finland!D24="","",Finland!D24)</f>
-        <v>_TKU</v>
+        <v>TKU</v>
       </c>
       <c r="D21" t="str">
         <f>IF(Finland!E24="","",Finland!E24)</f>
@@ -41327,7 +41327,7 @@
       </c>
       <c r="C22" t="str">
         <f>IF(Finland!D25="","",Finland!D25)</f>
-        <v>_TRE</v>
+        <v>TRE</v>
       </c>
       <c r="D22" t="str">
         <f>IF(Finland!E25="","",Finland!E25)</f>
@@ -41357,7 +41357,7 @@
       </c>
       <c r="C23" t="str">
         <f>IF(Finland!D26="","",Finland!D26)</f>
-        <v>_OUL</v>
+        <v>OUL</v>
       </c>
       <c r="D23" t="str">
         <f>IF(Finland!E26="","",Finland!E26)</f>
@@ -41387,7 +41387,7 @@
       </c>
       <c r="C24" t="str">
         <f>IF(Finland!D27="","",Finland!D27)</f>
-        <v>_JKL</v>
+        <v>JKL</v>
       </c>
       <c r="D24" t="str">
         <f>IF(Finland!E27="","",Finland!E27)</f>
@@ -41417,7 +41417,7 @@
       </c>
       <c r="C25" t="str">
         <f>IF(Finland!D28="","",Finland!D28)</f>
-        <v>_ROF</v>
+        <v>ROF</v>
       </c>
       <c r="D25" t="str">
         <f>IF(Finland!E28="","",Finland!E28)</f>
@@ -41447,7 +41447,7 @@
       </c>
       <c r="C26" t="str">
         <f>IF(Finland!D29="","",Finland!D29)</f>
-        <v>_HKI</v>
+        <v>HKI</v>
       </c>
       <c r="D26" t="str">
         <f>IF(Finland!E29="","",Finland!E29)</f>
@@ -41477,7 +41477,7 @@
       </c>
       <c r="C27" t="str">
         <f>IF(Finland!D30="","",Finland!D30)</f>
-        <v>_ESP</v>
+        <v>ESP</v>
       </c>
       <c r="D27" t="str">
         <f>IF(Finland!E30="","",Finland!E30)</f>
@@ -41507,7 +41507,7 @@
       </c>
       <c r="C28" t="str">
         <f>IF(Finland!D31="","",Finland!D31)</f>
-        <v>_VAN</v>
+        <v>VAN</v>
       </c>
       <c r="D28" t="str">
         <f>IF(Finland!E31="","",Finland!E31)</f>
@@ -41537,7 +41537,7 @@
       </c>
       <c r="C29" t="str">
         <f>IF(Finland!D32="","",Finland!D32)</f>
-        <v>_TKU</v>
+        <v>TKU</v>
       </c>
       <c r="D29" t="str">
         <f>IF(Finland!E32="","",Finland!E32)</f>
@@ -41567,7 +41567,7 @@
       </c>
       <c r="C30" t="str">
         <f>IF(Finland!D33="","",Finland!D33)</f>
-        <v>_TRE</v>
+        <v>TRE</v>
       </c>
       <c r="D30" t="str">
         <f>IF(Finland!E33="","",Finland!E33)</f>
@@ -41597,7 +41597,7 @@
       </c>
       <c r="C31" t="str">
         <f>IF(Finland!D34="","",Finland!D34)</f>
-        <v>_OUL</v>
+        <v>OUL</v>
       </c>
       <c r="D31" t="str">
         <f>IF(Finland!E34="","",Finland!E34)</f>
@@ -41627,7 +41627,7 @@
       </c>
       <c r="C32" t="str">
         <f>IF(Finland!D35="","",Finland!D35)</f>
-        <v>_JKL</v>
+        <v>JKL</v>
       </c>
       <c r="D32" t="str">
         <f>IF(Finland!E35="","",Finland!E35)</f>
@@ -41657,7 +41657,7 @@
       </c>
       <c r="C33" t="str">
         <f>IF(Finland!D36="","",Finland!D36)</f>
-        <v>_ROF</v>
+        <v>ROF</v>
       </c>
       <c r="D33" t="str">
         <f>IF(Finland!E36="","",Finland!E36)</f>
@@ -43494,7 +43494,7 @@
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="L27" sqref="L27"/>
-      <selection pane="topRight" activeCell="D35" sqref="D35"/>
+      <selection pane="topRight" activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -43552,7 +43552,7 @@
         <v>175</v>
       </c>
       <c r="G4" s="67" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="H4" s="68" t="s">
         <v>176</v>
@@ -43563,10 +43563,10 @@
         <v>177</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D5" s="70" t="s">
-        <v>297</v>
+        <v>345</v>
       </c>
       <c r="E5" s="70" t="s">
         <v>179</v>
@@ -43600,10 +43600,10 @@
         <v>177</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D6" s="75" t="s">
-        <v>298</v>
+        <v>346</v>
       </c>
       <c r="E6" s="75" t="s">
         <v>179</v>
@@ -43620,7 +43620,7 @@
         <v>0.1889210674010644</v>
       </c>
       <c r="L6" s="122" t="s">
-        <v>297</v>
+        <v>345</v>
       </c>
       <c r="M6" s="110">
         <f>SUMIFS(AD$48:AD$105, $A$48:$A$105,$L6,    $C$48:$C$105,"Produced DH")</f>
@@ -43644,10 +43644,10 @@
         <v>177</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D7" s="70" t="s">
-        <v>299</v>
+        <v>347</v>
       </c>
       <c r="E7" s="70" t="s">
         <v>179</v>
@@ -43664,7 +43664,7 @@
         <v>0.1889210674010644</v>
       </c>
       <c r="L7" s="122" t="s">
-        <v>298</v>
+        <v>346</v>
       </c>
       <c r="M7" s="110">
         <f t="shared" ref="M7:M13" si="4">SUMIFS(AD$48:AD$105, $A$48:$A$105,$L7,    $C$48:$C$105,"Produced DH")</f>
@@ -43688,10 +43688,10 @@
         <v>177</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D8" s="75" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E8" s="75" t="s">
         <v>179</v>
@@ -43708,7 +43708,7 @@
         <v>0.1889210674010644</v>
       </c>
       <c r="L8" s="122" t="s">
-        <v>299</v>
+        <v>347</v>
       </c>
       <c r="M8" s="110">
         <f t="shared" si="4"/>
@@ -43732,10 +43732,10 @@
         <v>177</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D9" s="70" t="s">
-        <v>300</v>
+        <v>349</v>
       </c>
       <c r="E9" s="70" t="s">
         <v>179</v>
@@ -43752,7 +43752,7 @@
         <v>0.1889210674010644</v>
       </c>
       <c r="L9" s="122" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="M9" s="110">
         <f t="shared" si="4"/>
@@ -43776,10 +43776,10 @@
         <v>177</v>
       </c>
       <c r="C10" s="75" t="s">
+        <v>344</v>
+      </c>
+      <c r="D10" s="75" t="s">
         <v>350</v>
-      </c>
-      <c r="D10" s="75" t="s">
-        <v>301</v>
       </c>
       <c r="E10" s="75" t="s">
         <v>179</v>
@@ -43796,7 +43796,7 @@
         <v>0.1889210674010644</v>
       </c>
       <c r="L10" s="122" t="s">
-        <v>300</v>
+        <v>349</v>
       </c>
       <c r="M10" s="110">
         <f t="shared" si="4"/>
@@ -43820,10 +43820,10 @@
         <v>177</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D11" s="70" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E11" s="70" t="s">
         <v>179</v>
@@ -43840,7 +43840,7 @@
         <v>0.1889210674010644</v>
       </c>
       <c r="L11" s="122" t="s">
-        <v>301</v>
+        <v>350</v>
       </c>
       <c r="M11" s="110">
         <f t="shared" si="4"/>
@@ -43864,10 +43864,10 @@
         <v>177</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D12" s="75" t="s">
-        <v>302</v>
+        <v>352</v>
       </c>
       <c r="E12" s="75" t="s">
         <v>179</v>
@@ -43884,7 +43884,7 @@
         <v>0.1889210674010644</v>
       </c>
       <c r="L12" s="122" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M12" s="110">
         <f t="shared" si="4"/>
@@ -43908,10 +43908,10 @@
         <v>177</v>
       </c>
       <c r="C13" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D13" s="70" t="s">
-        <v>297</v>
+        <v>345</v>
       </c>
       <c r="E13" s="70" t="s">
         <v>179</v>
@@ -43929,7 +43929,7 @@
         <v>0.1889210674010644</v>
       </c>
       <c r="L13" s="122" t="s">
-        <v>302</v>
+        <v>352</v>
       </c>
       <c r="M13" s="110">
         <f t="shared" si="4"/>
@@ -43953,10 +43953,10 @@
         <v>177</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D14" s="75" t="s">
-        <v>298</v>
+        <v>346</v>
       </c>
       <c r="E14" s="75" t="s">
         <v>179</v>
@@ -43979,10 +43979,10 @@
         <v>177</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D15" s="70" t="s">
-        <v>299</v>
+        <v>347</v>
       </c>
       <c r="E15" s="70" t="s">
         <v>179</v>
@@ -44005,10 +44005,10 @@
         <v>177</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D16" s="75" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E16" s="75" t="s">
         <v>179</v>
@@ -44031,10 +44031,10 @@
         <v>177</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D17" s="70" t="s">
-        <v>300</v>
+        <v>349</v>
       </c>
       <c r="E17" s="70" t="s">
         <v>179</v>
@@ -44057,10 +44057,10 @@
         <v>177</v>
       </c>
       <c r="C18" s="75" t="s">
+        <v>344</v>
+      </c>
+      <c r="D18" s="75" t="s">
         <v>350</v>
-      </c>
-      <c r="D18" s="75" t="s">
-        <v>301</v>
       </c>
       <c r="E18" s="75" t="s">
         <v>179</v>
@@ -44083,10 +44083,10 @@
         <v>177</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D19" s="70" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E19" s="70" t="s">
         <v>179</v>
@@ -44109,10 +44109,10 @@
         <v>177</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D20" s="75" t="s">
-        <v>302</v>
+        <v>352</v>
       </c>
       <c r="E20" s="75" t="s">
         <v>179</v>
@@ -44135,10 +44135,10 @@
         <v>177</v>
       </c>
       <c r="C21" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D21" s="70" t="s">
-        <v>297</v>
+        <v>345</v>
       </c>
       <c r="E21" s="70" t="s">
         <v>179</v>
@@ -44161,10 +44161,10 @@
         <v>177</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D22" s="75" t="s">
-        <v>298</v>
+        <v>346</v>
       </c>
       <c r="E22" s="75" t="s">
         <v>179</v>
@@ -44187,10 +44187,10 @@
         <v>177</v>
       </c>
       <c r="C23" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D23" s="70" t="s">
-        <v>299</v>
+        <v>347</v>
       </c>
       <c r="E23" s="70" t="s">
         <v>179</v>
@@ -44213,10 +44213,10 @@
         <v>177</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D24" s="75" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E24" s="75" t="s">
         <v>179</v>
@@ -44239,10 +44239,10 @@
         <v>177</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D25" s="70" t="s">
-        <v>300</v>
+        <v>349</v>
       </c>
       <c r="E25" s="70" t="s">
         <v>179</v>
@@ -44265,10 +44265,10 @@
         <v>177</v>
       </c>
       <c r="C26" s="75" t="s">
+        <v>344</v>
+      </c>
+      <c r="D26" s="75" t="s">
         <v>350</v>
-      </c>
-      <c r="D26" s="75" t="s">
-        <v>301</v>
       </c>
       <c r="E26" s="75" t="s">
         <v>179</v>
@@ -44291,10 +44291,10 @@
         <v>177</v>
       </c>
       <c r="C27" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D27" s="70" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E27" s="70" t="s">
         <v>179</v>
@@ -44317,10 +44317,10 @@
         <v>177</v>
       </c>
       <c r="C28" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D28" s="75" t="s">
-        <v>302</v>
+        <v>352</v>
       </c>
       <c r="E28" s="75" t="s">
         <v>179</v>
@@ -44343,10 +44343,10 @@
         <v>177</v>
       </c>
       <c r="C29" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D29" s="70" t="s">
-        <v>297</v>
+        <v>345</v>
       </c>
       <c r="E29" s="70" t="s">
         <v>179</v>
@@ -44369,10 +44369,10 @@
         <v>177</v>
       </c>
       <c r="C30" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D30" s="75" t="s">
-        <v>298</v>
+        <v>346</v>
       </c>
       <c r="E30" s="75" t="s">
         <v>179</v>
@@ -44395,10 +44395,10 @@
         <v>177</v>
       </c>
       <c r="C31" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D31" s="70" t="s">
-        <v>299</v>
+        <v>347</v>
       </c>
       <c r="E31" s="70" t="s">
         <v>179</v>
@@ -44421,10 +44421,10 @@
         <v>177</v>
       </c>
       <c r="C32" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D32" s="75" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E32" s="75" t="s">
         <v>179</v>
@@ -44447,10 +44447,10 @@
         <v>177</v>
       </c>
       <c r="C33" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D33" s="70" t="s">
-        <v>300</v>
+        <v>349</v>
       </c>
       <c r="E33" s="70" t="s">
         <v>179</v>
@@ -44473,10 +44473,10 @@
         <v>177</v>
       </c>
       <c r="C34" s="75" t="s">
+        <v>344</v>
+      </c>
+      <c r="D34" s="75" t="s">
         <v>350</v>
-      </c>
-      <c r="D34" s="75" t="s">
-        <v>301</v>
       </c>
       <c r="E34" s="75" t="s">
         <v>179</v>
@@ -44499,10 +44499,10 @@
         <v>177</v>
       </c>
       <c r="C35" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D35" s="70" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E35" s="70" t="s">
         <v>179</v>
@@ -44525,10 +44525,10 @@
         <v>177</v>
       </c>
       <c r="C36" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D36" s="75" t="s">
-        <v>302</v>
+        <v>352</v>
       </c>
       <c r="E36" s="75" t="s">
         <v>179</v>
@@ -45024,7 +45024,7 @@
     </row>
     <row r="54" spans="1:37">
       <c r="A54" s="108" t="s">
-        <v>297</v>
+        <v>345</v>
       </c>
       <c r="B54" s="108" t="s">
         <v>91</v>
@@ -45132,7 +45132,7 @@
     <row r="55" spans="1:37">
       <c r="A55" s="108" t="str">
         <f t="shared" ref="A55" si="12">A54</f>
-        <v>_HKI</v>
+        <v>HKI</v>
       </c>
       <c r="B55" s="108" t="str">
         <f t="shared" ref="B55" si="13">B54</f>
@@ -45259,7 +45259,7 @@
     <row r="56" spans="1:37">
       <c r="A56" s="108" t="str">
         <f t="shared" ref="A56" si="14">A55</f>
-        <v>_HKI</v>
+        <v>HKI</v>
       </c>
       <c r="B56" s="108" t="str">
         <f t="shared" ref="B56" si="15">B55</f>
@@ -45389,7 +45389,7 @@
     <row r="57" spans="1:37">
       <c r="A57" s="108" t="str">
         <f t="shared" ref="A57:A58" si="16">A56</f>
-        <v>_HKI</v>
+        <v>HKI</v>
       </c>
       <c r="B57" s="108" t="str">
         <f t="shared" ref="B57:B58" si="17">B56</f>
@@ -45483,14 +45483,14 @@
     <row r="58" spans="1:37">
       <c r="A58" s="108" t="str">
         <f t="shared" si="16"/>
-        <v>_HKI</v>
+        <v>HKI</v>
       </c>
       <c r="B58" s="108" t="str">
         <f t="shared" si="17"/>
         <v>Helsinki</v>
       </c>
       <c r="C58" s="59" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D58" s="138"/>
       <c r="J58" s="112">
@@ -45623,7 +45623,7 @@
     </row>
     <row r="61" spans="1:37">
       <c r="A61" s="108" t="s">
-        <v>298</v>
+        <v>346</v>
       </c>
       <c r="B61" s="108" t="s">
         <v>92</v>
@@ -45731,7 +45731,7 @@
     <row r="62" spans="1:37">
       <c r="A62" s="108" t="str">
         <f t="shared" ref="A62:A65" si="39">A61</f>
-        <v>_ESP</v>
+        <v>ESP</v>
       </c>
       <c r="B62" s="108" t="str">
         <f t="shared" ref="B62:B65" si="40">B61</f>
@@ -45858,7 +45858,7 @@
     <row r="63" spans="1:37">
       <c r="A63" s="108" t="str">
         <f t="shared" si="39"/>
-        <v>_ESP</v>
+        <v>ESP</v>
       </c>
       <c r="B63" s="108" t="str">
         <f t="shared" si="40"/>
@@ -45988,7 +45988,7 @@
     <row r="64" spans="1:37">
       <c r="A64" s="108" t="str">
         <f t="shared" si="39"/>
-        <v>_ESP</v>
+        <v>ESP</v>
       </c>
       <c r="B64" s="108" t="str">
         <f t="shared" si="40"/>
@@ -46082,14 +46082,14 @@
     <row r="65" spans="1:50">
       <c r="A65" s="108" t="str">
         <f t="shared" si="39"/>
-        <v>_ESP</v>
+        <v>ESP</v>
       </c>
       <c r="B65" s="108" t="str">
         <f t="shared" si="40"/>
         <v>Espoo</v>
       </c>
       <c r="C65" s="59" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D65" s="138"/>
       <c r="J65" s="112">
@@ -46202,7 +46202,7 @@
     </row>
     <row r="68" spans="1:50">
       <c r="A68" s="108" t="s">
-        <v>299</v>
+        <v>347</v>
       </c>
       <c r="B68" s="108" t="s">
         <v>93</v>
@@ -46310,7 +46310,7 @@
     <row r="69" spans="1:50">
       <c r="A69" s="108" t="str">
         <f t="shared" ref="A69:A72" si="45">A68</f>
-        <v>_VAN</v>
+        <v>VAN</v>
       </c>
       <c r="B69" s="108" t="str">
         <f t="shared" ref="B69:B72" si="46">B68</f>
@@ -46437,7 +46437,7 @@
     <row r="70" spans="1:50">
       <c r="A70" s="108" t="str">
         <f t="shared" si="45"/>
-        <v>_VAN</v>
+        <v>VAN</v>
       </c>
       <c r="B70" s="108" t="str">
         <f t="shared" si="46"/>
@@ -46567,7 +46567,7 @@
     <row r="71" spans="1:50">
       <c r="A71" s="108" t="str">
         <f t="shared" si="45"/>
-        <v>_VAN</v>
+        <v>VAN</v>
       </c>
       <c r="B71" s="108" t="str">
         <f t="shared" si="46"/>
@@ -46661,14 +46661,14 @@
     <row r="72" spans="1:50">
       <c r="A72" s="108" t="str">
         <f t="shared" si="45"/>
-        <v>_VAN</v>
+        <v>VAN</v>
       </c>
       <c r="B72" s="108" t="str">
         <f t="shared" si="46"/>
         <v>Vantaa</v>
       </c>
       <c r="C72" s="59" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D72" s="138"/>
       <c r="J72" s="112">
@@ -46774,7 +46774,7 @@
     </row>
     <row r="75" spans="1:50">
       <c r="A75" s="108" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B75" s="108" t="s">
         <v>94</v>
@@ -46882,7 +46882,7 @@
     <row r="76" spans="1:50">
       <c r="A76" s="108" t="str">
         <f t="shared" ref="A76:A79" si="68">A75</f>
-        <v>_TKU</v>
+        <v>TKU</v>
       </c>
       <c r="B76" s="108" t="str">
         <f t="shared" ref="B76:B79" si="69">B75</f>
@@ -47009,7 +47009,7 @@
     <row r="77" spans="1:50">
       <c r="A77" s="108" t="str">
         <f t="shared" si="68"/>
-        <v>_TKU</v>
+        <v>TKU</v>
       </c>
       <c r="B77" s="108" t="str">
         <f t="shared" si="69"/>
@@ -47142,7 +47142,7 @@
     <row r="78" spans="1:50">
       <c r="A78" s="108" t="str">
         <f t="shared" si="68"/>
-        <v>_TKU</v>
+        <v>TKU</v>
       </c>
       <c r="B78" s="108" t="str">
         <f t="shared" si="69"/>
@@ -47236,14 +47236,14 @@
     <row r="79" spans="1:50">
       <c r="A79" s="108" t="str">
         <f t="shared" si="68"/>
-        <v>_TKU</v>
+        <v>TKU</v>
       </c>
       <c r="B79" s="108" t="str">
         <f t="shared" si="69"/>
         <v>Turku</v>
       </c>
       <c r="C79" s="59" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D79" s="138"/>
       <c r="J79" s="112">
@@ -47342,7 +47342,7 @@
     </row>
     <row r="82" spans="1:37">
       <c r="A82" s="108" t="s">
-        <v>300</v>
+        <v>349</v>
       </c>
       <c r="B82" s="108" t="s">
         <v>95</v>
@@ -47449,7 +47449,7 @@
     <row r="83" spans="1:37">
       <c r="A83" s="108" t="str">
         <f t="shared" ref="A83:A86" si="91">A82</f>
-        <v>_TRE</v>
+        <v>TRE</v>
       </c>
       <c r="B83" s="108" t="str">
         <f t="shared" ref="B83:B86" si="92">B82</f>
@@ -47576,7 +47576,7 @@
     <row r="84" spans="1:37">
       <c r="A84" s="108" t="str">
         <f t="shared" si="91"/>
-        <v>_TRE</v>
+        <v>TRE</v>
       </c>
       <c r="B84" s="108" t="str">
         <f t="shared" si="92"/>
@@ -47706,7 +47706,7 @@
     <row r="85" spans="1:37">
       <c r="A85" s="108" t="str">
         <f t="shared" si="91"/>
-        <v>_TRE</v>
+        <v>TRE</v>
       </c>
       <c r="B85" s="108" t="str">
         <f t="shared" si="92"/>
@@ -47800,14 +47800,14 @@
     <row r="86" spans="1:37">
       <c r="A86" s="108" t="str">
         <f t="shared" si="91"/>
-        <v>_TRE</v>
+        <v>TRE</v>
       </c>
       <c r="B86" s="108" t="str">
         <f t="shared" si="92"/>
         <v>Tampere</v>
       </c>
       <c r="C86" s="59" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D86" s="138"/>
       <c r="J86" s="112">
@@ -47906,7 +47906,7 @@
     </row>
     <row r="89" spans="1:37">
       <c r="A89" s="108" t="s">
-        <v>301</v>
+        <v>350</v>
       </c>
       <c r="B89" s="108" t="s">
         <v>96</v>
@@ -48013,7 +48013,7 @@
     <row r="90" spans="1:37">
       <c r="A90" s="108" t="str">
         <f t="shared" ref="A90:A93" si="114">A89</f>
-        <v>_OUL</v>
+        <v>OUL</v>
       </c>
       <c r="B90" s="108" t="str">
         <f t="shared" ref="B90:B93" si="115">B89</f>
@@ -48140,7 +48140,7 @@
     <row r="91" spans="1:37">
       <c r="A91" s="108" t="str">
         <f t="shared" si="114"/>
-        <v>_OUL</v>
+        <v>OUL</v>
       </c>
       <c r="B91" s="108" t="str">
         <f t="shared" si="115"/>
@@ -48270,7 +48270,7 @@
     <row r="92" spans="1:37">
       <c r="A92" s="108" t="str">
         <f t="shared" si="114"/>
-        <v>_OUL</v>
+        <v>OUL</v>
       </c>
       <c r="B92" s="108" t="str">
         <f t="shared" si="115"/>
@@ -48364,14 +48364,14 @@
     <row r="93" spans="1:37">
       <c r="A93" s="108" t="str">
         <f t="shared" si="114"/>
-        <v>_OUL</v>
+        <v>OUL</v>
       </c>
       <c r="B93" s="108" t="str">
         <f t="shared" si="115"/>
         <v>Oulu</v>
       </c>
       <c r="C93" s="59" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D93" s="138"/>
       <c r="J93" s="112">
@@ -48470,7 +48470,7 @@
     </row>
     <row r="96" spans="1:37">
       <c r="A96" s="108" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B96" s="108" t="s">
         <v>97</v>
@@ -48577,7 +48577,7 @@
     <row r="97" spans="1:37">
       <c r="A97" s="108" t="str">
         <f t="shared" ref="A97:A100" si="137">A96</f>
-        <v>_JKL</v>
+        <v>JKL</v>
       </c>
       <c r="B97" s="108" t="str">
         <f t="shared" ref="B97:B100" si="138">B96</f>
@@ -48704,7 +48704,7 @@
     <row r="98" spans="1:37">
       <c r="A98" s="108" t="str">
         <f t="shared" si="137"/>
-        <v>_JKL</v>
+        <v>JKL</v>
       </c>
       <c r="B98" s="108" t="str">
         <f t="shared" si="138"/>
@@ -48834,7 +48834,7 @@
     <row r="99" spans="1:37">
       <c r="A99" s="108" t="str">
         <f t="shared" si="137"/>
-        <v>_JKL</v>
+        <v>JKL</v>
       </c>
       <c r="B99" s="108" t="str">
         <f t="shared" si="138"/>
@@ -48928,14 +48928,14 @@
     <row r="100" spans="1:37">
       <c r="A100" s="108" t="str">
         <f t="shared" si="137"/>
-        <v>_JKL</v>
+        <v>JKL</v>
       </c>
       <c r="B100" s="108" t="str">
         <f t="shared" si="138"/>
         <v>Jyväskylä</v>
       </c>
       <c r="C100" s="59" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D100" s="138"/>
       <c r="J100" s="112">
@@ -49034,7 +49034,7 @@
     </row>
     <row r="103" spans="1:37">
       <c r="A103" s="108" t="s">
-        <v>302</v>
+        <v>352</v>
       </c>
       <c r="B103" s="108" t="s">
         <v>294</v>
@@ -49141,7 +49141,7 @@
     <row r="104" spans="1:37">
       <c r="A104" s="108" t="str">
         <f t="shared" ref="A104:A107" si="160">A103</f>
-        <v>_ROF</v>
+        <v>ROF</v>
       </c>
       <c r="B104" s="108" t="str">
         <f t="shared" ref="B104:B107" si="161">B103</f>
@@ -49268,7 +49268,7 @@
     <row r="105" spans="1:37">
       <c r="A105" s="108" t="str">
         <f t="shared" si="160"/>
-        <v>_ROF</v>
+        <v>ROF</v>
       </c>
       <c r="B105" s="108" t="str">
         <f t="shared" si="161"/>
@@ -49398,7 +49398,7 @@
     <row r="106" spans="1:37">
       <c r="A106" s="108" t="str">
         <f t="shared" si="160"/>
-        <v>_ROF</v>
+        <v>ROF</v>
       </c>
       <c r="B106" s="108" t="str">
         <f t="shared" si="161"/>
@@ -49492,14 +49492,14 @@
     <row r="107" spans="1:37">
       <c r="A107" s="108" t="str">
         <f t="shared" si="160"/>
-        <v>_ROF</v>
+        <v>ROF</v>
       </c>
       <c r="B107" s="108" t="str">
         <f t="shared" si="161"/>
         <v>Rest of Finland</v>
       </c>
       <c r="C107" s="59" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D107" s="138"/>
       <c r="J107" s="112">
@@ -51681,7 +51681,7 @@
         <v>175</v>
       </c>
       <c r="G4" s="67" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="H4" s="68" t="s">
         <v>176</v>
@@ -51692,7 +51692,7 @@
         <v>167</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D5" s="70"/>
       <c r="E5" s="70" t="s">
@@ -51721,7 +51721,7 @@
         <v>168</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D6" s="75"/>
       <c r="E6" s="75" t="s">
@@ -51751,7 +51751,7 @@
         <v>169</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D7" s="70"/>
       <c r="E7" s="70" t="s">
@@ -51781,7 +51781,7 @@
         <v>167</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D8" s="75"/>
       <c r="E8" s="75" t="s">
@@ -51811,7 +51811,7 @@
         <v>168</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70" t="s">
@@ -51834,7 +51834,7 @@
         <v>169</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D10" s="75"/>
       <c r="E10" s="75" t="s">
@@ -51869,7 +51869,7 @@
         <v>167</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70" t="s">
@@ -51911,7 +51911,7 @@
         <v>168</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D12" s="75"/>
       <c r="E12" s="75" t="s">
@@ -51934,7 +51934,7 @@
         <v>169</v>
       </c>
       <c r="C13" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D13" s="70"/>
       <c r="E13" s="70" t="s">
@@ -51957,7 +51957,7 @@
         <v>167</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D14" s="75"/>
       <c r="E14" s="75" t="s">
@@ -51980,7 +51980,7 @@
         <v>168</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70" t="s">
@@ -52006,7 +52006,7 @@
         <v>169</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D16" s="75"/>
       <c r="E16" s="75" t="s">
@@ -55053,7 +55053,7 @@
         <v>175</v>
       </c>
       <c r="G4" s="67" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="H4" s="68" t="s">
         <v>176</v>
@@ -55064,7 +55064,7 @@
         <v>189</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D5" s="70"/>
       <c r="E5" s="70" t="s">
@@ -55089,7 +55089,7 @@
         <v>194</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D6" s="75"/>
       <c r="E6" s="75" t="s">
@@ -55112,7 +55112,7 @@
         <v>207</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D7" s="70"/>
       <c r="E7" s="70" t="s">
@@ -55141,7 +55141,7 @@
         <v>212</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D8" s="75"/>
       <c r="E8" s="75" t="s">
@@ -55175,7 +55175,7 @@
         <v>189</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70" t="s">
@@ -55210,7 +55210,7 @@
         <v>194</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D10" s="75"/>
       <c r="E10" s="75" t="s">
@@ -55247,7 +55247,7 @@
         <v>207</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70" t="s">
@@ -55282,7 +55282,7 @@
         <v>212</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D12" s="75"/>
       <c r="E12" s="75" t="s">
@@ -55306,7 +55306,7 @@
         <v>189</v>
       </c>
       <c r="C13" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D13" s="70"/>
       <c r="E13" s="70" t="s">
@@ -55330,7 +55330,7 @@
         <v>194</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D14" s="75"/>
       <c r="E14" s="75" t="s">
@@ -55366,7 +55366,7 @@
         <v>207</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70" t="s">
@@ -55409,7 +55409,7 @@
         <v>212</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D16" s="75"/>
       <c r="E16" s="75" t="s">
@@ -55433,7 +55433,7 @@
         <v>189</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D17" s="70"/>
       <c r="E17" s="70" t="s">
@@ -55457,7 +55457,7 @@
         <v>194</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D18" s="75"/>
       <c r="E18" s="75" t="s">
@@ -55481,7 +55481,7 @@
         <v>207</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D19" s="70"/>
       <c r="E19" s="70" t="s">
@@ -55505,7 +55505,7 @@
         <v>212</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D20" s="75"/>
       <c r="E20" s="75" t="s">
@@ -57852,7 +57852,7 @@
         <v>175</v>
       </c>
       <c r="G4" s="67" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="H4" s="68" t="s">
         <v>176</v>
@@ -57866,7 +57866,7 @@
         <v>239</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D5" s="70"/>
       <c r="E5" s="70" t="s">
@@ -57904,7 +57904,7 @@
         <v>240</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D6" s="75"/>
       <c r="E6" s="75" t="s">
@@ -57946,7 +57946,7 @@
         <v>239</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D7" s="70"/>
       <c r="E7" s="70" t="s">
@@ -57989,7 +57989,7 @@
         <v>240</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D8" s="75"/>
       <c r="E8" s="75" t="s">
@@ -58013,7 +58013,7 @@
         <v>239</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70" t="s">
@@ -58037,7 +58037,7 @@
         <v>240</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D10" s="75"/>
       <c r="E10" s="75" t="s">
@@ -58073,7 +58073,7 @@
         <v>239</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70" t="s">
@@ -58116,7 +58116,7 @@
         <v>240</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D12" s="75"/>
       <c r="E12" s="75" t="s">
@@ -60678,7 +60678,7 @@
         <v>175</v>
       </c>
       <c r="G4" s="67" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="H4" s="68" t="s">
         <v>176</v>
@@ -60698,10 +60698,10 @@
     </row>
     <row r="5" spans="2:18">
       <c r="B5" s="69" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D5" s="70"/>
       <c r="E5" s="70" t="s">
@@ -60723,7 +60723,7 @@
         <v>Germany</v>
       </c>
       <c r="L5" s="46" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="M5">
         <v>99899.252443847246</v>
@@ -60745,10 +60745,10 @@
     </row>
     <row r="6" spans="2:18">
       <c r="B6" s="74" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D6" s="75"/>
       <c r="E6" s="75" t="s">
@@ -60770,7 +60770,7 @@
         <v>Germany</v>
       </c>
       <c r="L6" s="46" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="M6">
         <v>106034.24989443528</v>
@@ -60792,10 +60792,10 @@
     </row>
     <row r="7" spans="2:18">
       <c r="B7" s="69" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D7" s="70"/>
       <c r="E7" s="70" t="s">
@@ -60817,7 +60817,7 @@
         <v>Germany</v>
       </c>
       <c r="L7" s="46" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="M7">
         <v>8198.8831734358682</v>
@@ -60839,10 +60839,10 @@
     </row>
     <row r="8" spans="2:18">
       <c r="B8" s="74" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D8" s="75"/>
       <c r="E8" s="75" t="s">
@@ -60864,7 +60864,7 @@
         <v>Germany</v>
       </c>
       <c r="L8" s="46" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="M8">
         <v>7529.8520086006029</v>
@@ -60886,10 +60886,10 @@
     </row>
     <row r="9" spans="2:18">
       <c r="B9" s="69" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70" t="s">
@@ -60911,7 +60911,7 @@
         <v>Poland</v>
       </c>
       <c r="L9" s="46" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="M9">
         <v>10363.858136581519</v>
@@ -60933,10 +60933,10 @@
     </row>
     <row r="10" spans="2:18">
       <c r="B10" s="74" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D10" s="75"/>
       <c r="E10" s="75" t="s">
@@ -60958,7 +60958,7 @@
         <v>Poland</v>
       </c>
       <c r="L10" s="46" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="M10">
         <v>5305.6507823887514</v>
@@ -60980,10 +60980,10 @@
     </row>
     <row r="11" spans="2:18">
       <c r="B11" s="69" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70" t="s">
@@ -61007,10 +61007,10 @@
     </row>
     <row r="12" spans="2:18">
       <c r="B12" s="74" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D12" s="75"/>
       <c r="E12" s="75" t="s">
@@ -61034,10 +61034,10 @@
     </row>
     <row r="13" spans="2:18">
       <c r="B13" s="70" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C13" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D13" s="70"/>
       <c r="E13" s="70" t="s">
@@ -61061,10 +61061,10 @@
     </row>
     <row r="14" spans="2:18">
       <c r="B14" s="75" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D14" s="75"/>
       <c r="E14" s="75" t="s">
@@ -61088,10 +61088,10 @@
     </row>
     <row r="15" spans="2:18">
       <c r="B15" s="70" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70" t="s">
@@ -61115,10 +61115,10 @@
     </row>
     <row r="16" spans="2:18">
       <c r="B16" s="75" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D16" s="75"/>
       <c r="E16" s="75" t="s">
@@ -61142,10 +61142,10 @@
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="70" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D17" s="70"/>
       <c r="E17" s="70" t="s">
@@ -61169,10 +61169,10 @@
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="75" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D18" s="75"/>
       <c r="E18" s="75" t="s">
@@ -61196,10 +61196,10 @@
     </row>
     <row r="19" spans="2:10">
       <c r="B19" s="70" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D19" s="70"/>
       <c r="E19" s="70" t="s">
@@ -61223,10 +61223,10 @@
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="75" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D20" s="75"/>
       <c r="E20" s="75" t="s">
@@ -61250,10 +61250,10 @@
     </row>
     <row r="21" spans="2:10">
       <c r="B21" s="70" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C21" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D21" s="70"/>
       <c r="E21" s="70" t="s">
@@ -61277,10 +61277,10 @@
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="75" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D22" s="75"/>
       <c r="E22" s="75" t="s">
@@ -61304,10 +61304,10 @@
     </row>
     <row r="23" spans="2:10">
       <c r="B23" s="70" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C23" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D23" s="70"/>
       <c r="E23" s="70" t="s">
@@ -61331,10 +61331,10 @@
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="75" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D24" s="75"/>
       <c r="E24" s="75" t="s">
@@ -61358,10 +61358,10 @@
     </row>
     <row r="25" spans="2:10">
       <c r="B25" s="70" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D25" s="70"/>
       <c r="E25" s="70" t="s">
@@ -61385,10 +61385,10 @@
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="75" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C26" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D26" s="75"/>
       <c r="E26" s="75" t="s">
@@ -61412,10 +61412,10 @@
     </row>
     <row r="27" spans="2:10">
       <c r="B27" s="70" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C27" s="70" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D27" s="70"/>
       <c r="E27" s="70" t="s">
@@ -61439,10 +61439,10 @@
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="75" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C28" s="75" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D28" s="75"/>
       <c r="E28" s="75" t="s">

</xml_diff>